<commit_message>
updated analyses to focus on native herbivores only
</commit_message>
<xml_diff>
--- a/Beetle Data_2020_Final.xlsx
+++ b/Beetle Data_2020_Final.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01C624A-66EE-4660-9B2D-97747927A2F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF5A581-52B2-4175-A383-BD76E9C4F523}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-7200" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2259" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2260" uniqueCount="497">
   <si>
     <t>Block</t>
   </si>
@@ -1791,6 +1791,9 @@
   <si>
     <t>C</t>
   </si>
+  <si>
+    <t>not collected via bark/spray</t>
+  </si>
 </sst>
 </file>
 
@@ -1876,7 +1879,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1898,6 +1901,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1952,7 +1961,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2036,6 +2045,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14621,13 +14631,13 @@
   <dimension ref="A1:CV126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
@@ -15248,6 +15258,9 @@
       </c>
     </row>
     <row r="3" spans="1:100" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="B3" s="49" t="s">
+        <v>496</v>
+      </c>
       <c r="I3" s="3" t="s">
         <v>5</v>
       </c>
@@ -15894,7 +15907,7 @@
       <c r="AM5" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="AN5" s="2" t="s">
+      <c r="AN5" s="49" t="s">
         <v>428</v>
       </c>
       <c r="AO5" s="2" t="s">
@@ -15999,7 +16012,7 @@
       <c r="BV5" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="BW5" s="2" t="s">
+      <c r="BW5" s="49" t="s">
         <v>463</v>
       </c>
       <c r="BX5" s="2" t="s">
@@ -52739,5 +52752,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>